<commit_message>
Subsets >= 9, cleaning, merging in DL models and labeling
</commit_message>
<xml_diff>
--- a/cleaning/normalisasi.xlsx
+++ b/cleaning/normalisasi.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salmadanu/Desktop/Skripsi/skripsi-env/narasipal/cleaning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5A992D-B6B1-C84B-9890-3D995E74D8E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BC4ACD-B48D-3946-A2D2-C604FB163B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11300" yWindow="500" windowWidth="21700" windowHeight="15500" xr2:uid="{A5ED81BA-20F2-494E-86FC-3174948FB482}"/>
+    <workbookView xWindow="3900" yWindow="500" windowWidth="21700" windowHeight="15500" activeTab="3" xr2:uid="{A5ED81BA-20F2-494E-86FC-3174948FB482}"/>
   </bookViews>
   <sheets>
     <sheet name="normalisasi" sheetId="1" r:id="rId1"/>
     <sheet name="remove" sheetId="2" r:id="rId2"/>
+    <sheet name="stemming" sheetId="3" r:id="rId3"/>
+    <sheet name="NER" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
   <si>
     <t>before</t>
   </si>
@@ -83,9 +85,6 @@
     <t>dubes</t>
   </si>
   <si>
-    <t>rs</t>
-  </si>
-  <si>
     <t>rumah sakit</t>
   </si>
   <si>
@@ -131,9 +130,6 @@
     <t>korea utara</t>
   </si>
   <si>
-    <t>koresel</t>
-  </si>
-  <si>
     <t>korea selatan</t>
   </si>
   <si>
@@ -170,12 +166,6 @@
     <t xml:space="preserve"> eks </t>
   </si>
   <si>
-    <t xml:space="preserve"> vs </t>
-  </si>
-  <si>
-    <t>versus</t>
-  </si>
-  <si>
     <t>kemlu</t>
   </si>
   <si>
@@ -194,9 +184,6 @@
     <t xml:space="preserve"> ri-</t>
   </si>
   <si>
-    <t>Indonesia</t>
-  </si>
-  <si>
     <t xml:space="preserve"> arab saudi </t>
   </si>
   <si>
@@ -237,6 +224,54 @@
   </si>
   <si>
     <t>bunuh</t>
+  </si>
+  <si>
+    <t>hezbollah</t>
+  </si>
+  <si>
+    <t>hizbullah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-as </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-ri </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rs </t>
+  </si>
+  <si>
+    <t>palestine</t>
+  </si>
+  <si>
+    <t>palestina</t>
+  </si>
+  <si>
+    <t>korsel</t>
+  </si>
+  <si>
+    <t>asia</t>
+  </si>
+  <si>
+    <t>asian</t>
+  </si>
+  <si>
+    <t>kurbo</t>
+  </si>
+  <si>
+    <t>kubro</t>
+  </si>
+  <si>
+    <t>pengungsian</t>
+  </si>
+  <si>
+    <t>pengungsi</t>
+  </si>
+  <si>
+    <t>israel</t>
+  </si>
+  <si>
+    <t>gaza</t>
   </si>
 </sst>
 </file>
@@ -598,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7278BC78-5F5E-F94B-A460-2EBF2685323D}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,7 +655,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -628,7 +663,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -676,7 +711,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
@@ -692,186 +727,226 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>47</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>66</v>
+      <c r="B35" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -884,44 +959,105 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7405065-3011-FC4E-87E7-56568B015FA9}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC555A1-BBE6-0D43-B812-ED4B268B9919}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>